<commit_message>
Rename naif_id as reg_id. Add confusing id check. Update based on decisions in 2024-01-24 meeting.
</commit_message>
<xml_diff>
--- a/test/reader/dong_ying/output.xlsx
+++ b/test/reader/dong_ying/output.xlsx
@@ -56,8 +56,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I179"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,47 +455,87 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>142701</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>43910</v>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Y185809趙</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>185403</v>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>有問題</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>44609</v>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Y182801德</t>
+          <t>Y121005地</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>無登</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>趙德</t>
-        </is>
+          <t>Y146101趙</t>
+        </is>
+      </c>
+      <c r="G1" t="n">
+        <v>244310</v>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>母/公</t>
+          <t>地趙</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>['"性別 母/公 錯誤。性別需定義於下表：\\n{\'公\': \'M\', \'母\': \'F\', \'M\': \'M\', \'F\': \'F\', \'1\': \'M\', \'2\': \'F\'}"']</t>
+          <t>母</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>['不允許有相近耳號']</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="H2" s="2" t="n"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>188003</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>L?</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44665</v>
+      </c>
+      <c r="E2" t="n">
+        <v/>
+      </c>
+      <c r="F2" t="n">
+        <v/>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>無登</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v/>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>母</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>['不允許有相近耳號']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -506,42 +546,84 @@
       <c r="B3" t="n">
         <v>190202</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" t="n">
+        <v/>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>44705</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Y155009合</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Y126104地</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" s="1" t="inlineStr">
         <is>
           <t>????</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>????</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>母</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>['登錄號不能含有非數字字元 ']</t>
         </is>
       </c>
     </row>
-    <row r="179">
-      <c r="F179" s="2" t="n"/>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>137105</v>
+      </c>
+      <c r="C4" t="n">
+        <v>137108</v>
+      </c>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Y195207王</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Y182001趙</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>238789</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>王趙</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>母</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>['需要有子代的生日才能設定親代', '需要有子代的生日才能設定親代', '不允許有相近耳號']</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>